<commit_message>
change in ticl_chase_weekly_report module
</commit_message>
<xml_diff>
--- a/ticl_import/sample_file/update_stock_status.xlsx
+++ b/ticl_import/sample_file/update_stock_status.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t xml:space="preserve">Unique ID</t>
   </si>
@@ -28,37 +28,28 @@
     <t xml:space="preserve">status</t>
   </si>
   <si>
-    <t xml:space="preserve">1066</t>
+    <t xml:space="preserve">21795</t>
   </si>
   <si>
     <t xml:space="preserve">shipped</t>
   </si>
   <si>
-    <t xml:space="preserve">1065</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1064</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1063</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1056</t>
+    <t xml:space="preserve">21796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21792</t>
   </si>
   <si>
     <t xml:space="preserve">sold</t>
   </si>
   <si>
-    <t xml:space="preserve">1057</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1058</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1059</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1060</t>
+    <t xml:space="preserve">21957</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21956</t>
   </si>
 </sst>
 </file>
@@ -70,7 +61,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -91,6 +82,17 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,7 +137,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -152,12 +154,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -177,22 +187,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="27.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="10.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="8" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="10.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="6" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -203,88 +211,60 @@
         <v>1</v>
       </c>
       <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="0"/>
-      <c r="G2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
+      <c r="B7" s="5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>